<commit_message>
changed name sheets & added sheet
from ThuThapYeuCau to YeuCauTongQuat and added ThuThapYeuCau (google form)
</commit_message>
<xml_diff>
--- a/QLDA_TiemBachHoaHaiTuiMinh.xlsx
+++ b/QLDA_TiemBachHoaHaiTuiMinh.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AD6354-295E-4FD4-86B4-CD90670EF15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C5A1E8-528A-4A34-AE01-DE7B107AFE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{26449352-15BB-4EDF-A4FC-8953C10D4408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{26449352-15BB-4EDF-A4FC-8953C10D4408}"/>
   </bookViews>
   <sheets>
     <sheet name="XacDinhDuAn" sheetId="1" r:id="rId1"/>
     <sheet name="KeHoach" sheetId="2" r:id="rId2"/>
-    <sheet name="ThuThapYeuCau" sheetId="3" r:id="rId3"/>
-    <sheet name="PhanTichTinhNang" sheetId="4" r:id="rId4"/>
+    <sheet name="ThuThapYeuCau" sheetId="5" r:id="rId3"/>
+    <sheet name="YeuCauTongQuat" sheetId="3" r:id="rId4"/>
+    <sheet name="PhanTichTinhNang" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="303">
   <si>
     <t>Tên dự án</t>
   </si>
@@ -1124,12 +1125,396 @@
   <si>
     <t>API nội bộ cho mobile app</t>
   </si>
+  <si>
+    <t>Yêu cầu tổng quát (dự án)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Xây dựng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>website bán hàng bách hóa trực tuyến</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> với giao diện thân thiện, dễ dùng.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Website cần có </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>chức năng mua sắm online cơ bản</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (xem sản phẩm, tìm kiếm, giỏ hàng, thanh toán, quản lý tài khoản).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tích hợp </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>phương thức thanh toán đa dạng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (tiền mặt, chuyển khoản, ví điện tử).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Có </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>hệ thống quản trị cho admin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> để quản lý sản phẩm, khách hàng, đơn hàng.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hỗ trợ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>responsive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (PC, tablet, mobile).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dữ liệu sản phẩm, khách hàng, đơn hàng được quản lý tập trung bằng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CSDL MySQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Có thể mở rộng trong tương lai: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>API cho mobile app, chatbot AI, gợi ý sản phẩm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dấu thời gian</t>
+  </si>
+  <si>
+    <t>1. Bạn bao nhiêu tuổi?</t>
+  </si>
+  <si>
+    <t>2. Nghề nghiệp của bạn là gì?</t>
+  </si>
+  <si>
+    <t>3. Bạn có thường xuyên mua hàng bách hóa không?</t>
+  </si>
+  <si>
+    <t>4. Bạn thường mua hàng bách hóa ở đâu?</t>
+  </si>
+  <si>
+    <t>5. Bạn thường mua những loại sản phẩm nào?</t>
+  </si>
+  <si>
+    <t>6. Bạn chi trung bình bao nhiêu tiền/tháng cho bách hóa?</t>
+  </si>
+  <si>
+    <t>7. Khi mua hàng online, bạn quan tâm điều gì nhất?</t>
+  </si>
+  <si>
+    <t>8. Bạn có muốn được tích hợp thanh toán trực tuyến (Momo, VNPay, Banking)?</t>
+  </si>
+  <si>
+    <t>9. Bạn có muốn hệ thống gợi ý sản phẩm dựa trên lịch sử mua sắm của mình không?</t>
+  </si>
+  <si>
+    <t>10. Bạn có mong muốn có chatbot hỗ trợ khi gặp vấn đề?</t>
+  </si>
+  <si>
+    <t>11. Bạn có mong muốn gì thêm cho một website bách hóa online?</t>
+  </si>
+  <si>
+    <t>Từ 18-25 tuổi</t>
+  </si>
+  <si>
+    <t>Học sinh, sinh viên</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>Siêu thị, Cửa hàng tạp hóa, Online (Shopee, Lazada, Tiktok, Bách Hóa Xanh,..)</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ gia dụng, Đồ dùng cá nhân, Mỹ phẩm, Nhu yếu phẩm khác</t>
+  </si>
+  <si>
+    <t>Dưới 500k</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Khuyến mãi/voucher, Thời gian giao hàng</t>
+  </si>
+  <si>
+    <t>Khum</t>
+  </si>
+  <si>
+    <t>Dưới 18 tuổi</t>
+  </si>
+  <si>
+    <t>Cửa hàng tạp hóa, Online (Shopee, Lazada, Tiktok, Bách Hóa Xanh,..)</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ dùng cá nhân, Mỹ phẩm</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm</t>
+  </si>
+  <si>
+    <t>đa dạng hàng hóa, mẫu mã hơn, ...</t>
+  </si>
+  <si>
+    <t>Nhân viên văn phòng</t>
+  </si>
+  <si>
+    <t>Online (Shopee, Lazada, Tiktok, Bách Hóa Xanh,..)</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ gia dụng, Đồ dùng cá nhân, Mỹ phẩm, Vệ sinh nhà cửa, Nhu yếu phẩm khác</t>
+  </si>
+  <si>
+    <t>Trên 2 triệu</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Khuyến mãi/voucher, Thời gian giao hàng, Đa dạng sản phẩm</t>
+  </si>
+  <si>
+    <t>Thông tin so rõ ràng cụ thể</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Đồ dùng cá nhân</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Khuyến mãi/voucher</t>
+  </si>
+  <si>
+    <t>Ko</t>
+  </si>
+  <si>
+    <t>Từ 500k-1 triệu</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Khuyến mãi/voucher, Đa dạng sản phẩm, tính ứng dụng của sản phẩm</t>
+  </si>
+  <si>
+    <t>không</t>
+  </si>
+  <si>
+    <t>Từ 25-40 tuổi</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ gia dụng, Đồ dùng cá nhân, Mỹ phẩm, Vệ sinh nhà cửa</t>
+  </si>
+  <si>
+    <t>Chất lượng sản phẩm</t>
+  </si>
+  <si>
+    <t>Không có</t>
+  </si>
+  <si>
+    <t>Công việc tự do</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ gia dụng, Đồ dùng cá nhân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hình ảnh thực tế của sản phẩm
+- Có sẵn đầy đủ các loại mặt hàng (Size, loại hàng, màu sắc,...)
+- Có nhân viên CSKH trả lời nhanh khi có khách hỏi về sản phẩm mà không phải đợi thời gian dài 
+</t>
+  </si>
+  <si>
+    <t>25/09/2025 2:22:37</t>
+  </si>
+  <si>
+    <t>Kinh doanh</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ gia dụng, Đồ dùng cá nhân, Vệ sinh nhà cửa, Nhu yếu phẩm khác</t>
+  </si>
+  <si>
+    <t>Từ 1-2 triệu</t>
+  </si>
+  <si>
+    <t>Chất lượng sản phẩm, Khuyến mãi/voucher, Thời gian giao hàng, Đa dạng sản phẩm</t>
+  </si>
+  <si>
+    <t>Cập nhật thông tin sản phẩm mới</t>
+  </si>
+  <si>
+    <t>Trên 40 tuổi</t>
+  </si>
+  <si>
+    <t>Giáo viên</t>
+  </si>
+  <si>
+    <t>Cửa hàng tạp hóa</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ dùng cá nhân, Vệ sinh nhà cửa, Nhu yếu phẩm khác</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Khuyến mãi/voucher, Đa dạng sản phẩm</t>
+  </si>
+  <si>
+    <t>Hàng đảm bảo chất lượng và vệ sinh an toàn thực phẩm</t>
+  </si>
+  <si>
+    <t>Mỹ phẩm</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>ăn ở không</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ dùng cá nhân</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Thời gian giao hàng</t>
+  </si>
+  <si>
+    <t>Siêu thị, Cửa hàng tạp hóa</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống</t>
+  </si>
+  <si>
+    <t>Chất lượng sản phẩm, Khuyến mãi/voucher, Thời gian giao hàng</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Nhu yếu phẩm khác</t>
+  </si>
+  <si>
+    <t>Giá cả, Chất lượng sản phẩm, Khuyến mãi/voucher, Thời gian giao hàng, Đa dạng sản phẩm,</t>
+  </si>
+  <si>
+    <t>Thực phẩm, Đồ uống, Đồ gia dụng, Mỹ phẩm</t>
+  </si>
+  <si>
+    <t>khôngg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1230,8 +1615,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF434343"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1274,8 +1678,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B3F86"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1335,12 +1757,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF5B3F86"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF442F65"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF5B3F86"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF442F65"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF442F65"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1406,6 +1993,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1457,12 +2050,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1505,6 +2092,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1513,6 +2103,51 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="17" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="17" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="17" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1850,12 +2485,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="2" t="s">
         <v>100</v>
       </c>
@@ -1873,13 +2508,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="25" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="27" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1896,11 +2531,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="26"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1915,11 +2550,11 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1930,12 +2565,12 @@
       <c r="I4" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -1944,501 +2579,501 @@
       <c r="A7" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="23"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="23"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="41"/>
+      <c r="D9" s="23"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="41"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="23"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="41"/>
+      <c r="D11" s="23"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
-      <c r="B12" s="40"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="41"/>
+      <c r="D12" s="23"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
-      <c r="B13" s="40"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="41"/>
+      <c r="D13" s="23"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
-      <c r="B14" s="40"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="23"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
-      <c r="B15" s="40"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="23"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="23"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
-      <c r="B17" s="40"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="23"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
-      <c r="B18" s="40"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="23"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
-      <c r="B19" s="40"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="23"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
-      <c r="B20" s="40"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="23"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="23"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
-      <c r="B22" s="40"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="23"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="23"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="23"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
-      <c r="B25" s="40"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="23"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
-      <c r="B26" s="40"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="41"/>
+      <c r="D26" s="23"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
-      <c r="B27" s="40"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="23"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="41"/>
+      <c r="D28" s="23"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
-      <c r="B29" s="40"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="23"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
-      <c r="B30" s="40"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="41"/>
+      <c r="D30" s="23"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
-      <c r="B31" s="40"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="41"/>
+      <c r="D31" s="23"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
-      <c r="B32" s="40"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="41"/>
+      <c r="D32" s="23"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="40" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="41"/>
+      <c r="D33" s="23"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="49"/>
-      <c r="B34" s="38"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="41"/>
+      <c r="D34" s="23"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
-      <c r="B35" s="38"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="41"/>
+      <c r="D35" s="23"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
-      <c r="B36" s="38"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="41"/>
+      <c r="D36" s="23"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
-      <c r="B37" s="38"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="41"/>
+      <c r="D37" s="23"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49"/>
-      <c r="B38" s="38"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="41"/>
+      <c r="D38" s="23"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
-      <c r="B39" s="38"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="41"/>
+      <c r="D39" s="23"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="40" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="41"/>
+      <c r="D40" s="23"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49"/>
-      <c r="B41" s="38"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="41"/>
+      <c r="D41" s="23"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
-      <c r="B42" s="38"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="41"/>
+      <c r="D42" s="23"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="49"/>
-      <c r="B43" s="38"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="41"/>
+      <c r="D43" s="23"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49"/>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="24" t="s">
         <v>56</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="41"/>
+      <c r="D44" s="23"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="49"/>
-      <c r="B45" s="40"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="41"/>
+      <c r="D45" s="23"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="49"/>
-      <c r="B46" s="40"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="41"/>
+      <c r="D46" s="23"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49"/>
-      <c r="B47" s="40"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="41"/>
+      <c r="D47" s="23"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49"/>
-      <c r="B48" s="40"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="41"/>
+      <c r="D48" s="23"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49"/>
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="24" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="41"/>
+      <c r="D49" s="23"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49"/>
-      <c r="B50" s="40"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="41"/>
+      <c r="D50" s="23"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49"/>
-      <c r="B51" s="40"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="41"/>
+      <c r="D51" s="23"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49"/>
-      <c r="B52" s="40"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="41"/>
+      <c r="D52" s="23"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49"/>
-      <c r="B53" s="40"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="41"/>
+      <c r="D53" s="23"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49"/>
-      <c r="B54" s="40"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="41"/>
+      <c r="D54" s="23"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="31" t="s">
         <v>150</v>
       </c>
       <c r="C55" s="13" t="s">
@@ -2450,8 +3085,8 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="49"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="32" t="s">
+      <c r="B56" s="32"/>
+      <c r="C56" s="34" t="s">
         <v>152</v>
       </c>
       <c r="D56" s="3" t="s">
@@ -2462,8 +3097,8 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="49"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="33"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="3" t="s">
         <v>158</v>
       </c>
@@ -2472,8 +3107,8 @@
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="33"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="3" t="s">
         <v>85</v>
       </c>
@@ -2482,8 +3117,8 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="49"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="33"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="3" t="s">
         <v>10</v>
       </c>
@@ -2492,8 +3127,8 @@
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="49"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="33"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="3" t="s">
         <v>159</v>
       </c>
@@ -2502,8 +3137,8 @@
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="49"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="34"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="36"/>
       <c r="D61" s="19" t="s">
         <v>203</v>
       </c>
@@ -2512,37 +3147,37 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="49"/>
-      <c r="B62" s="30"/>
+      <c r="B62" s="32"/>
       <c r="C62" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D62" s="35"/>
+      <c r="D62" s="37"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="49"/>
-      <c r="B63" s="30"/>
+      <c r="B63" s="32"/>
       <c r="C63" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D63" s="36"/>
+      <c r="D63" s="38"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="49"/>
-      <c r="B64" s="30"/>
+      <c r="B64" s="32"/>
       <c r="C64" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D64" s="37"/>
+      <c r="D64" s="39"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="49"/>
-      <c r="B65" s="30"/>
+      <c r="B65" s="32"/>
       <c r="C65" s="13" t="s">
         <v>153</v>
       </c>
@@ -2552,7 +3187,7 @@
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="49"/>
-      <c r="B66" s="30"/>
+      <c r="B66" s="32"/>
       <c r="C66" s="13" t="s">
         <v>154</v>
       </c>
@@ -2562,7 +3197,7 @@
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="49"/>
-      <c r="B67" s="30"/>
+      <c r="B67" s="32"/>
       <c r="C67" s="13" t="s">
         <v>156</v>
       </c>
@@ -2572,7 +3207,7 @@
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="49"/>
-      <c r="B68" s="31"/>
+      <c r="B68" s="33"/>
       <c r="C68" s="13" t="s">
         <v>155</v>
       </c>
@@ -2582,10 +3217,10 @@
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="49"/>
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="32" t="s">
+      <c r="C69" s="34" t="s">
         <v>161</v>
       </c>
       <c r="D69" s="3" t="s">
@@ -2596,8 +3231,8 @@
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="49"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="33"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="35"/>
       <c r="D70" s="3" t="s">
         <v>163</v>
       </c>
@@ -2606,8 +3241,8 @@
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="49"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="33"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="35"/>
       <c r="D71" s="3" t="s">
         <v>164</v>
       </c>
@@ -2616,8 +3251,8 @@
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="34"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="36"/>
       <c r="D72" s="3" t="s">
         <v>165</v>
       </c>
@@ -2626,7 +3261,7 @@
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="49"/>
-      <c r="B73" s="30"/>
+      <c r="B73" s="32"/>
       <c r="C73" s="13" t="s">
         <v>166</v>
       </c>
@@ -2638,7 +3273,7 @@
     </row>
     <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="50"/>
-      <c r="B74" s="31"/>
+      <c r="B74" s="33"/>
       <c r="C74" s="13" t="s">
         <v>155</v>
       </c>
@@ -2650,40 +3285,40 @@
       <c r="A75" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B75" s="38" t="s">
+      <c r="B75" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D75" s="35"/>
+      <c r="D75" s="37"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49"/>
-      <c r="B76" s="38"/>
+      <c r="B76" s="40"/>
       <c r="C76" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="36"/>
+      <c r="D76" s="38"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49"/>
-      <c r="B77" s="38"/>
+      <c r="B77" s="40"/>
       <c r="C77" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D77" s="37"/>
+      <c r="D77" s="39"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="39" t="s">
+      <c r="B78" s="40"/>
+      <c r="C78" s="41" t="s">
         <v>69</v>
       </c>
       <c r="D78" s="3" t="s">
@@ -2694,8 +3329,8 @@
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="39"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="41"/>
       <c r="D79" s="3" t="s">
         <v>11</v>
       </c>
@@ -2704,8 +3339,8 @@
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="39"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="41"/>
       <c r="D80" s="3" t="s">
         <v>10</v>
       </c>
@@ -2714,8 +3349,8 @@
     </row>
     <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="39"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="41"/>
       <c r="D81" s="3" t="s">
         <v>84</v>
       </c>
@@ -2724,8 +3359,8 @@
     </row>
     <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="49"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="39"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="41"/>
       <c r="D82" s="3" t="s">
         <v>85</v>
       </c>
@@ -2734,8 +3369,8 @@
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="49"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="39"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="41"/>
       <c r="D83" s="3" t="s">
         <v>86</v>
       </c>
@@ -2744,60 +3379,60 @@
     </row>
     <row r="84" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="49"/>
-      <c r="B84" s="38"/>
+      <c r="B84" s="40"/>
       <c r="C84" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="41"/>
+      <c r="D84" s="23"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="49"/>
-      <c r="B85" s="38" t="s">
+      <c r="B85" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D85" s="41"/>
+      <c r="D85" s="23"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="49"/>
-      <c r="B86" s="38"/>
+      <c r="B86" s="40"/>
       <c r="C86" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D86" s="41"/>
+      <c r="D86" s="23"/>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
     </row>
     <row r="87" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="49"/>
-      <c r="B87" s="38"/>
+      <c r="B87" s="40"/>
       <c r="C87" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D87" s="41"/>
+      <c r="D87" s="23"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="49"/>
-      <c r="B88" s="38"/>
+      <c r="B88" s="40"/>
       <c r="C88" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D88" s="41"/>
+      <c r="D88" s="23"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="49"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="39" t="s">
+      <c r="B89" s="40"/>
+      <c r="C89" s="41" t="s">
         <v>37</v>
       </c>
       <c r="D89" s="3" t="s">
@@ -2808,8 +3443,8 @@
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="49"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="39"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="41"/>
       <c r="D90" s="3" t="s">
         <v>88</v>
       </c>
@@ -2818,8 +3453,8 @@
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="49"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="39"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="41"/>
       <c r="D91" s="3" t="s">
         <v>89</v>
       </c>
@@ -2828,8 +3463,8 @@
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="49"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="39" t="s">
+      <c r="B92" s="40"/>
+      <c r="C92" s="41" t="s">
         <v>28</v>
       </c>
       <c r="D92" s="3" t="s">
@@ -2840,8 +3475,8 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="49"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="39"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="41"/>
       <c r="D93" s="3" t="s">
         <v>91</v>
       </c>
@@ -2850,8 +3485,8 @@
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="49"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="39"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="41"/>
       <c r="D94" s="3" t="s">
         <v>92</v>
       </c>
@@ -2860,102 +3495,102 @@
     </row>
     <row r="95" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="49"/>
-      <c r="B95" s="38"/>
+      <c r="B95" s="40"/>
       <c r="C95" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D95" s="41"/>
+      <c r="D95" s="23"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="49"/>
-      <c r="B96" s="38" t="s">
+      <c r="B96" s="40" t="s">
         <v>39</v>
       </c>
       <c r="C96" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D96" s="41"/>
+      <c r="D96" s="23"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
     </row>
     <row r="97" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="49"/>
-      <c r="B97" s="38"/>
+      <c r="B97" s="40"/>
       <c r="C97" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D97" s="41"/>
+      <c r="D97" s="23"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
     </row>
     <row r="98" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="49"/>
-      <c r="B98" s="38"/>
+      <c r="B98" s="40"/>
       <c r="C98" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D98" s="41"/>
+      <c r="D98" s="23"/>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
     </row>
     <row r="99" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="49"/>
-      <c r="B99" s="38"/>
+      <c r="B99" s="40"/>
       <c r="C99" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D99" s="41"/>
+      <c r="D99" s="23"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
     <row r="100" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="49"/>
-      <c r="B100" s="38"/>
+      <c r="B100" s="40"/>
       <c r="C100" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D100" s="41"/>
+      <c r="D100" s="23"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
     <row r="101" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="49"/>
-      <c r="B101" s="38"/>
+      <c r="B101" s="40"/>
       <c r="C101" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D101" s="41"/>
+      <c r="D101" s="23"/>
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
     </row>
     <row r="102" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="49"/>
-      <c r="B102" s="38" t="s">
+      <c r="B102" s="40" t="s">
         <v>77</v>
       </c>
       <c r="C102" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D102" s="41"/>
+      <c r="D102" s="23"/>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
     </row>
     <row r="103" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="49"/>
-      <c r="B103" s="38"/>
+      <c r="B103" s="40"/>
       <c r="C103" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D103" s="41"/>
+      <c r="D103" s="23"/>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
     <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="49"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="39" t="s">
+      <c r="B104" s="40"/>
+      <c r="C104" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D104" s="3" t="s">
@@ -2966,8 +3601,8 @@
     </row>
     <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="49"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="39"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="41"/>
       <c r="D105" s="3" t="s">
         <v>10</v>
       </c>
@@ -2976,8 +3611,8 @@
     </row>
     <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="50"/>
-      <c r="B106" s="38"/>
-      <c r="C106" s="39"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="41"/>
       <c r="D106" s="3" t="s">
         <v>95</v>
       </c>
@@ -3523,7 +4158,7 @@
       <c r="F157" s="47"/>
     </row>
     <row r="159" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="28" t="s">
+      <c r="A159" s="30" t="s">
         <v>145</v>
       </c>
       <c r="B159" s="18" t="s">
@@ -3534,7 +4169,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="28"/>
+      <c r="A160" s="30"/>
       <c r="B160" s="18" t="s">
         <v>147</v>
       </c>
@@ -3586,6 +4221,20 @@
     <mergeCell ref="B96:B101"/>
     <mergeCell ref="B102:B106"/>
     <mergeCell ref="C104:C106"/>
+    <mergeCell ref="C78:C83"/>
+    <mergeCell ref="B75:B84"/>
+    <mergeCell ref="D126:G129"/>
+    <mergeCell ref="D117:G121"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C130:C133"/>
+    <mergeCell ref="D130:G133"/>
+    <mergeCell ref="A159:A160"/>
+    <mergeCell ref="B55:B68"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="C56:C61"/>
     <mergeCell ref="A110:A138"/>
     <mergeCell ref="B110:B116"/>
     <mergeCell ref="B117:B138"/>
@@ -3596,36 +4245,22 @@
     <mergeCell ref="D137:G137"/>
     <mergeCell ref="D138:G138"/>
     <mergeCell ref="D134:G134"/>
-    <mergeCell ref="D126:G129"/>
-    <mergeCell ref="D117:G121"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="C130:C133"/>
-    <mergeCell ref="D130:G133"/>
-    <mergeCell ref="C78:C83"/>
-    <mergeCell ref="B75:B84"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D7:D54"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A2:D4"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A159:A160"/>
-    <mergeCell ref="B55:B68"/>
-    <mergeCell ref="B69:B74"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="D62:D64"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C56:C61"/>
-    <mergeCell ref="D7:D54"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="B40:B43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{480B51DA-D2FC-46D1-85B4-1BA72886D70D}"/>
@@ -3812,23 +4447,809 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E5765F-581A-472A-9DB6-4362D1A4E6CC}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="B20" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="64" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="64" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="64" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" style="64" customWidth="1"/>
+    <col min="5" max="5" width="91.28515625" style="64" customWidth="1"/>
+    <col min="6" max="6" width="115" style="64" customWidth="1"/>
+    <col min="7" max="7" width="68.5703125" style="64" customWidth="1"/>
+    <col min="8" max="8" width="108.5703125" style="64" customWidth="1"/>
+    <col min="9" max="9" width="96" style="64" customWidth="1"/>
+    <col min="10" max="10" width="98.85546875" style="64" customWidth="1"/>
+    <col min="11" max="11" width="70.28515625" style="64" customWidth="1"/>
+    <col min="12" max="12" width="227.7109375" style="64" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="64"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="62" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="62" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="65">
+        <v>45924.995393518519</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="66" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="J2" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="L2" s="67" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="68">
+        <v>45925.001909722225</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>254</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="J3" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="K3" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="L3" s="70" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="65">
+        <v>45925.004710648151</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" s="66" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="J4" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="L4" s="67" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="68">
+        <v>45925.010289351849</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>265</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" s="69" t="s">
+        <v>266</v>
+      </c>
+      <c r="I5" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="J5" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="K5" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="L5" s="70" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="65">
+        <v>45925.016562500001</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="H6" s="66" t="s">
+        <v>269</v>
+      </c>
+      <c r="I6" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="J6" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="K6" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="L6" s="67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="68">
+        <v>45925.053483796299</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>272</v>
+      </c>
+      <c r="G7" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="H7" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="I7" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="J7" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="K7" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" s="70" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="65">
+        <v>45925.090405092589</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>276</v>
+      </c>
+      <c r="G8" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="H8" s="66" t="s">
+        <v>256</v>
+      </c>
+      <c r="I8" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="J8" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="L8" s="67" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="71" t="s">
+        <v>278</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>281</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>282</v>
+      </c>
+      <c r="I9" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="J9" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="K9" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="L9" s="70" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="65">
+        <v>45925.214699074073</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>286</v>
+      </c>
+      <c r="F10" s="66" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="H10" s="66" t="s">
+        <v>288</v>
+      </c>
+      <c r="I10" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="K10" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="L10" s="67" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="68">
+        <v>45925.534224537034</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="69" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>262</v>
+      </c>
+      <c r="I11" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="J11" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="K11" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="L11" s="70" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="65">
+        <v>45925.63858796296</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>292</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>286</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>293</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>294</v>
+      </c>
+      <c r="I12" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="K12" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="L12" s="67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="68">
+        <v>45925.674699074072</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>295</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>296</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="H13" s="69" t="s">
+        <v>297</v>
+      </c>
+      <c r="I13" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="J13" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="K13" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="L13" s="70" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="65">
+        <v>45925.977048611108</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>253</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>299</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="H14" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="I14" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="J14" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="L14" s="67" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="72">
+        <v>45926.251030092593</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" s="73" t="s">
+        <v>301</v>
+      </c>
+      <c r="G15" s="73" t="s">
+        <v>250</v>
+      </c>
+      <c r="H15" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="I15" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="J15" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="K15" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="L15" s="74" t="s">
+        <v>302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D976198E-F002-40A9-B011-1F76D0DE0075}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="A8:O8"/>
+    <mergeCell ref="A9:O9"/>
+    <mergeCell ref="A1:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A6:O6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F25EC64-B0B4-4B27-A596-1A7E09450898}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3839,291 +5260,285 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="58" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="58" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="58" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58" t="s">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58" t="s">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58" t="s">
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58" t="s">
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58" t="s">
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58" t="s">
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58" t="s">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58" t="s">
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="58" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="58" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="58" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="58" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="58" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E13:J13"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E16:J16"/>
     <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:D8"/>
     <mergeCell ref="A9:D14"/>
@@ -4134,6 +5549,12 @@
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>